<commit_message>
GPIO assignment changed to avoid external pull-up resistors.
</commit_message>
<xml_diff>
--- a/GPIO Assignment.xlsx
+++ b/GPIO Assignment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jabra4-my.sharepoint.com/personal/klisby_gnhearing_com/Documents/Desktop/src/train_elevator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F3F85F1-B8BA-4804-8FC1-7F0F32D83243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{8F3F85F1-B8BA-4804-8FC1-7F0F32D83243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1032F227-1048-40DB-8A6F-0591622FFB64}"/>
   <bookViews>
-    <workbookView xWindow="3610" yWindow="2410" windowWidth="22040" windowHeight="16730" xr2:uid="{9769F012-8B96-4717-94D0-9BF45318C815}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{9769F012-8B96-4717-94D0-9BF45318C815}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="37">
   <si>
     <t>GPIO</t>
   </si>
@@ -89,9 +89,6 @@
     <t>outputs PWM signal at boot</t>
   </si>
   <si>
-    <t>input only</t>
-  </si>
-  <si>
     <t>DCC in</t>
   </si>
   <si>
@@ -101,18 +98,6 @@
     <t>I2C Display SDA</t>
   </si>
   <si>
-    <t>SD card MOSI</t>
-  </si>
-  <si>
-    <t>SD Card MISO</t>
-  </si>
-  <si>
-    <t>SD Card SCK</t>
-  </si>
-  <si>
-    <t>SD Card CS</t>
-  </si>
-  <si>
     <t>Left Stepper Direction</t>
   </si>
   <si>
@@ -144,13 +129,31 @@
   </si>
   <si>
     <t>My pin assignment</t>
+  </si>
+  <si>
+    <t>Avaliable on 30-pin board</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>I2C SDA</t>
+  </si>
+  <si>
+    <t>I2C SCL</t>
+  </si>
+  <si>
+    <t>input only - no internal pullup</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -190,8 +193,86 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,8 +303,68 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FFCC0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED1C24"/>
+        <bgColor rgb="FFED1C24"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFADD58A"/>
+        <bgColor rgb="FFADD58A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFF200"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -353,24 +494,57 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF808080"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
+      <right style="thin">
+        <color rgb="FF808080"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF808080"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="9"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -417,12 +591,38 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="19">
+    <cellStyle name="Accent" xfId="8" xr:uid="{9CC2F021-D91D-47C8-A9B1-C41F27F2F12F}"/>
+    <cellStyle name="Accent 1" xfId="9" xr:uid="{CF4BE655-B93E-46E3-9931-5699D9C0B186}"/>
+    <cellStyle name="Accent 2" xfId="10" xr:uid="{90D9B83C-3FD1-49E5-BE52-0ADAA1D78241}"/>
+    <cellStyle name="Accent 3" xfId="11" xr:uid="{CE884EB7-5C20-48AA-A6E1-5377D6FD5A53}"/>
+    <cellStyle name="Bad 2" xfId="5" xr:uid="{B438F014-39A0-4E64-852F-D7916E4AFC30}"/>
+    <cellStyle name="Error" xfId="12" xr:uid="{E5CCCEA1-D727-494A-B976-5BD6AA137AE7}"/>
+    <cellStyle name="Footnote" xfId="13" xr:uid="{F1F88923-87AC-4949-974D-F070E1591F61}"/>
+    <cellStyle name="Good 2" xfId="4" xr:uid="{2B01EF82-EA3C-40E4-92A8-F4725ECC4A57}"/>
+    <cellStyle name="Heading" xfId="14" xr:uid="{63422177-0471-44CD-9AF2-34394A3EDB55}"/>
+    <cellStyle name="Heading 1 2" xfId="2" xr:uid="{CAEA88EC-FD0A-42DA-B07F-8416E8C6D897}"/>
+    <cellStyle name="Heading 2 2" xfId="3" xr:uid="{D322BC43-0048-4CB7-A4DC-0E01479FDE33}"/>
+    <cellStyle name="Hyperlink" xfId="15" xr:uid="{C59F0062-022F-459B-92ED-B8812DE49174}"/>
+    <cellStyle name="Neutral 2" xfId="6" xr:uid="{0258337B-DAF2-4178-9E60-6001289E164F}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{31093D0D-7CE6-47B2-A6D8-F083606095A0}"/>
+    <cellStyle name="Note 2" xfId="7" xr:uid="{B917120A-D045-410D-8A6A-1ECCC61622F7}"/>
+    <cellStyle name="Status" xfId="16" xr:uid="{922CF022-4FC3-4D44-9F56-CADF8C69AFC0}"/>
+    <cellStyle name="Text" xfId="17" xr:uid="{CD97ED75-6165-4A0B-AD25-1481ABCAA7BA}"/>
+    <cellStyle name="Warning" xfId="18" xr:uid="{CCAC2285-4E28-4E16-8C5F-C72460F353E5}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -438,9 +638,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -478,7 +678,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -584,7 +784,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -726,7 +926,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -734,19 +934,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090F0C66-1780-4B03-A7EE-C0104851A2CD}">
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:F179"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
     <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="55" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="36">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -757,13 +958,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+      <c r="F1" s="19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -777,8 +981,11 @@
       <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+      <c r="F2" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -792,8 +999,11 @@
       <c r="E3" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+      <c r="F3" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -807,8 +1017,11 @@
       <c r="E4" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+      <c r="F4" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -822,9 +1035,12 @@
       <c r="E5" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="F5" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="24">
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -833,11 +1049,16 @@
       <c r="C6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="F6" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="24">
         <v>5</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -846,15 +1067,16 @@
       <c r="C7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="D7" s="7"/>
       <c r="E7" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="F7" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="24">
         <v>6</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -867,9 +1089,12 @@
       <c r="E8" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="F8" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="24">
         <v>7</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -882,9 +1107,12 @@
       <c r="E9" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="F9" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="24">
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -897,9 +1125,12 @@
       <c r="E10" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="F10" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="24">
         <v>9</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -912,9 +1143,12 @@
       <c r="E11" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+      <c r="F11" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="24">
         <v>10</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -927,9 +1161,12 @@
       <c r="E12" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+      <c r="F12" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="24">
         <v>11</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -942,9 +1179,12 @@
       <c r="E13" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+      <c r="F13" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="24">
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -957,9 +1197,12 @@
       <c r="E14" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="F14" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="24">
         <v>13</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -970,9 +1213,12 @@
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+      <c r="F15" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="24">
         <v>14</v>
       </c>
       <c r="B16" s="10" t="s">
@@ -985,9 +1231,12 @@
       <c r="E16" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="F16" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="24">
         <v>15</v>
       </c>
       <c r="B17" s="10" t="s">
@@ -1000,9 +1249,12 @@
       <c r="E17" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+      <c r="F17" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="13.5" thickBot="1">
+      <c r="A18" s="24">
         <v>16</v>
       </c>
       <c r="B18" s="10" t="s">
@@ -1011,13 +1263,16 @@
       <c r="C18" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>30</v>
+      <c r="D18" s="17" t="s">
+        <v>28</v>
       </c>
       <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+      <c r="F18" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="24">
         <v>17</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -1030,9 +1285,12 @@
         <v>29</v>
       </c>
       <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+      <c r="F19" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="24">
         <v>18</v>
       </c>
       <c r="B20" s="10" t="s">
@@ -1042,86 +1300,108 @@
         <v>5</v>
       </c>
       <c r="D20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="24">
+        <v>19</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="24">
+        <v>21</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="24">
+        <v>22</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="24">
         <v>23</v>
       </c>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
-        <v>19</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
-        <v>21</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="7" t="s">
+      <c r="B24" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="24">
+        <v>25</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="11"/>
-    </row>
-    <row r="23" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
-        <v>22</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="11"/>
-    </row>
-    <row r="24" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
-        <v>23</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="11"/>
-    </row>
-    <row r="25" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
-        <v>25</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>25</v>
-      </c>
       <c r="E25" s="11"/>
-    </row>
-    <row r="26" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+      <c r="F25" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="5">
         <v>26</v>
       </c>
@@ -1132,11 +1412,14 @@
         <v>5</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E26" s="11"/>
-    </row>
-    <row r="27" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+      <c r="F26" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="5">
         <v>27</v>
       </c>
@@ -1147,11 +1430,14 @@
         <v>5</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E27" s="11"/>
-    </row>
-    <row r="28" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+      <c r="F27" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="5">
         <v>32</v>
       </c>
@@ -1162,11 +1448,14 @@
         <v>5</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E28" s="11"/>
-    </row>
-    <row r="29" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+      <c r="F28" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="5">
         <v>33</v>
       </c>
@@ -1177,11 +1466,14 @@
         <v>5</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E29" s="11"/>
-    </row>
-    <row r="30" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+      <c r="F29" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="5">
         <v>34</v>
       </c>
@@ -1189,14 +1481,15 @@
         <v>5</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="7" t="s">
-        <v>32</v>
-      </c>
+      <c r="D30" s="12"/>
       <c r="E30" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="5">
         <v>35</v>
       </c>
@@ -1204,14 +1497,15 @@
         <v>5</v>
       </c>
       <c r="C31" s="12"/>
-      <c r="D31" s="7" t="s">
-        <v>31</v>
-      </c>
+      <c r="D31" s="12"/>
       <c r="E31" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="5">
         <v>36</v>
       </c>
@@ -1219,14 +1513,15 @@
         <v>5</v>
       </c>
       <c r="C32" s="12"/>
-      <c r="D32" s="7" t="s">
-        <v>34</v>
-      </c>
+      <c r="D32" s="12"/>
       <c r="E32" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="F32" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="13.5" thickBot="1">
       <c r="A33" s="14">
         <v>39</v>
       </c>
@@ -1234,594 +1529,602 @@
         <v>5</v>
       </c>
       <c r="C33" s="16"/>
-      <c r="D33" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="16"/>
+      <c r="E33" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="22"/>
+    </row>
+    <row r="35" spans="1:6">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="22"/>
+    </row>
+    <row r="36" spans="1:6">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="22"/>
+    </row>
+    <row r="37" spans="1:6">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="22"/>
+    </row>
+    <row r="38" spans="1:6">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="22"/>
+    </row>
+    <row r="39" spans="1:6">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="22"/>
+    </row>
+    <row r="40" spans="1:6">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="22"/>
+    </row>
+    <row r="41" spans="1:6">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:3">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:3">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:3">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:3">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:3">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:3">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:3">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:3">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:3">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:3">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:3">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:3">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:3">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:3">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:3">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:3">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:3">
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:3">
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:3">
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:3">
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:3">
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:3">
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:3">
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:3">
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:3">
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:3">
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:3">
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:3">
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:3">
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:3">
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:3">
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:3">
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:3">
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:3">
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:3">
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:3">
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:3">
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:3">
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:3">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:3">
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:3">
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:3">
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:3">
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:3">
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:3">
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:3">
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:3">
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:3">
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:3">
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:3">
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:3">
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:3">
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:3">
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:3">
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:3">
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:3">
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:3">
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:3">
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:3">
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:3">
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:3">
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:3">
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
     </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:3">
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:3">
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:3">
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:3">
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
     </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:3">
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:3">
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
     </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:3">
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
     </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:3">
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
     </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:3">
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
     </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:3">
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
     </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:3">
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
     </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:3">
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
     </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:3">
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:3">
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:3">
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:3">
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:3">
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:3">
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:3">
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:3">
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:3">
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:3">
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
     </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:3">
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:3">
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
     </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:3">
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
     </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:3">
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
     </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:3">
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
     </row>
-    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:3">
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
     </row>
-    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:3">
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
     </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:3">
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
     </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:3">
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
     </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:3">
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
     </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:3">
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
     </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:3">
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
     </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:3">
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
     </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:3">
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
     </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:3">
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
     </row>
-    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:3">
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
     </row>
-    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:3">
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
     </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:3">
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
     </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:3">
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
     </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:3">
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
     </row>
-    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:3">
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
     </row>
-    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:3">
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
     </row>
-    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:3">
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
     </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:3">
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
     </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:3">
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
     </row>
-    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:3">
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
     </row>

</xml_diff>